<commit_message>
feat: módulo precificacao inicial
</commit_message>
<xml_diff>
--- a/cadastro_produtos_template.xlsx
+++ b/cadastro_produtos_template.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Apps\Datahive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A7051F9-5BA1-43DC-9DFB-C465A225FBB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B0410D4-00EB-4D3A-B5F9-DA4EF8274FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="produtos" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">produtos!$A$1:$AK$41</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -233,9 +236,6 @@
     <t>28.999.10</t>
   </si>
   <si>
-    <t>28.999.11</t>
-  </si>
-  <si>
     <t>28.999.12</t>
   </si>
   <si>
@@ -489,6 +489,9 @@
   </si>
   <si>
     <t>KIT 2X EXTRATO DE PRÓPOLIS CONCENTRADO 11% 20ML MELBRAS</t>
+  </si>
+  <si>
+    <t>28.062.00</t>
   </si>
 </sst>
 </file>
@@ -913,21 +916,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AK41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="G13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
+      <selection pane="bottomRight" activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" customWidth="1"/>
+    <col min="4" max="4" width="30" customWidth="1"/>
     <col min="5" max="5" width="9.28515625" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
@@ -949,10 +953,7 @@
     <col min="23" max="23" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13.28515625" customWidth="1"/>
-    <col min="26" max="26" width="10.5703125" customWidth="1"/>
-    <col min="27" max="27" width="10.7109375" customWidth="1"/>
-    <col min="28" max="28" width="9.7109375" customWidth="1"/>
-    <col min="29" max="29" width="16.7109375" customWidth="1"/>
+    <col min="26" max="29" width="22.140625" customWidth="1"/>
     <col min="30" max="30" width="16" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="22.28515625" bestFit="1" customWidth="1"/>
@@ -977,10 +978,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>3</v>
@@ -1010,7 +1011,7 @@
         <v>12</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>13</v>
@@ -1031,25 +1032,25 @@
         <v>18</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="X1" s="2" t="s">
         <v>19</v>
       </c>
       <c r="Y1" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AB1" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="Z1" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="AD1" s="2" t="s">
         <v>20</v>
@@ -1076,7 +1077,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>7898915380804</v>
       </c>
@@ -1090,7 +1091,7 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>52</v>
@@ -1123,7 +1124,7 @@
         <v>51</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
@@ -1153,7 +1154,7 @@
       </c>
       <c r="AE2" s="4"/>
       <c r="AF2" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AG2" s="4"/>
       <c r="AH2" s="4">
@@ -1163,7 +1164,7 @@
       <c r="AJ2" s="4"/>
       <c r="AK2" s="4"/>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>7898915380934</v>
       </c>
@@ -1177,7 +1178,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>52</v>
@@ -1210,7 +1211,7 @@
         <v>51</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="U3" s="4"/>
       <c r="V3" s="4"/>
@@ -1240,7 +1241,7 @@
       </c>
       <c r="AE3" s="4"/>
       <c r="AF3" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AG3" s="4"/>
       <c r="AH3" s="4">
@@ -1250,7 +1251,7 @@
       <c r="AJ3" s="4"/>
       <c r="AK3" s="4"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>7898915380927</v>
       </c>
@@ -1264,7 +1265,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>52</v>
@@ -1297,7 +1298,7 @@
         <v>51</v>
       </c>
       <c r="T4" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="U4" s="4"/>
       <c r="V4" s="4"/>
@@ -1327,7 +1328,7 @@
       </c>
       <c r="AE4" s="4"/>
       <c r="AF4" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AG4" s="4"/>
       <c r="AH4" s="4">
@@ -1337,7 +1338,7 @@
       <c r="AJ4" s="4"/>
       <c r="AK4" s="4"/>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>7898915380781</v>
       </c>
@@ -1384,7 +1385,7 @@
         <v>51</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="U5" s="4"/>
       <c r="V5" s="4"/>
@@ -1414,7 +1415,7 @@
       </c>
       <c r="AE5" s="4"/>
       <c r="AF5" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AG5" s="4"/>
       <c r="AH5" s="4">
@@ -1424,7 +1425,7 @@
       <c r="AJ5" s="4"/>
       <c r="AK5" s="4"/>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>7898915380958</v>
       </c>
@@ -1471,7 +1472,7 @@
         <v>51</v>
       </c>
       <c r="T6" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="U6" s="4"/>
       <c r="V6" s="4"/>
@@ -1501,7 +1502,7 @@
       </c>
       <c r="AE6" s="4"/>
       <c r="AF6" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AG6" s="4"/>
       <c r="AH6" s="4">
@@ -1511,7 +1512,7 @@
       <c r="AJ6" s="4"/>
       <c r="AK6" s="4"/>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>7898915380941</v>
       </c>
@@ -1558,7 +1559,7 @@
         <v>51</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
@@ -1588,7 +1589,7 @@
       </c>
       <c r="AE7" s="4"/>
       <c r="AF7" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AG7" s="4"/>
       <c r="AH7" s="4">
@@ -1598,7 +1599,7 @@
       <c r="AJ7" s="4"/>
       <c r="AK7" s="4"/>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7908883300213</v>
       </c>
@@ -1612,7 +1613,7 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>52</v>
@@ -1645,7 +1646,7 @@
         <v>51</v>
       </c>
       <c r="T8" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
@@ -1675,7 +1676,7 @@
       </c>
       <c r="AE8" s="4"/>
       <c r="AF8" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AG8" s="4"/>
       <c r="AH8" s="4">
@@ -1685,7 +1686,7 @@
       <c r="AJ8" s="4"/>
       <c r="AK8" s="4"/>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7908883300190</v>
       </c>
@@ -1699,7 +1700,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>52</v>
@@ -1732,7 +1733,7 @@
         <v>51</v>
       </c>
       <c r="T9" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U9" s="4"/>
       <c r="V9" s="4"/>
@@ -1762,7 +1763,7 @@
       </c>
       <c r="AE9" s="4"/>
       <c r="AF9" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AG9" s="4"/>
       <c r="AH9" s="4">
@@ -1772,7 +1773,7 @@
       <c r="AJ9" s="4"/>
       <c r="AK9" s="4"/>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>7908883300183</v>
       </c>
@@ -1786,7 +1787,7 @@
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>52</v>
@@ -1819,7 +1820,7 @@
         <v>51</v>
       </c>
       <c r="T10" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U10" s="4"/>
       <c r="V10" s="4"/>
@@ -1849,7 +1850,7 @@
       </c>
       <c r="AE10" s="4"/>
       <c r="AF10" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AG10" s="4"/>
       <c r="AH10" s="4">
@@ -1859,7 +1860,7 @@
       <c r="AJ10" s="4"/>
       <c r="AK10" s="4"/>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>7908883300206</v>
       </c>
@@ -1873,7 +1874,7 @@
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>52</v>
@@ -1906,7 +1907,7 @@
         <v>51</v>
       </c>
       <c r="T11" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="U11" s="4"/>
       <c r="V11" s="4"/>
@@ -1936,7 +1937,7 @@
       </c>
       <c r="AE11" s="4"/>
       <c r="AF11" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AG11" s="4"/>
       <c r="AH11" s="4">
@@ -1946,7 +1947,7 @@
       <c r="AJ11" s="4"/>
       <c r="AK11" s="4"/>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>7908883300244</v>
       </c>
@@ -1960,7 +1961,7 @@
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>52</v>
@@ -1993,7 +1994,7 @@
         <v>51</v>
       </c>
       <c r="T12" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="U12" s="4"/>
       <c r="V12" s="4"/>
@@ -2023,7 +2024,7 @@
       </c>
       <c r="AE12" s="4"/>
       <c r="AF12" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AG12" s="4"/>
       <c r="AH12" s="4">
@@ -2053,7 +2054,7 @@
         <v>17049020</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>66</v>
+        <v>151</v>
       </c>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
@@ -2078,7 +2079,7 @@
         <v>51</v>
       </c>
       <c r="T13" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="U13" s="4"/>
       <c r="V13" s="4"/>
@@ -2108,7 +2109,7 @@
       </c>
       <c r="AE13" s="4"/>
       <c r="AF13" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AG13" s="4"/>
       <c r="AH13" s="4">
@@ -2118,7 +2119,7 @@
       <c r="AJ13" s="4"/>
       <c r="AK13" s="4"/>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>7908883300152</v>
       </c>
@@ -2138,7 +2139,7 @@
         <v>17049020</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -2163,7 +2164,7 @@
         <v>51</v>
       </c>
       <c r="T14" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="U14" s="4"/>
       <c r="V14" s="4"/>
@@ -2193,7 +2194,7 @@
       </c>
       <c r="AE14" s="4"/>
       <c r="AF14" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AG14" s="4"/>
       <c r="AH14" s="4">
@@ -2203,7 +2204,7 @@
       <c r="AJ14" s="4"/>
       <c r="AK14" s="4"/>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>7908883300169</v>
       </c>
@@ -2223,7 +2224,7 @@
         <v>17049020</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
@@ -2248,7 +2249,7 @@
         <v>51</v>
       </c>
       <c r="T15" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="U15" s="4"/>
       <c r="V15" s="4"/>
@@ -2278,7 +2279,7 @@
       </c>
       <c r="AE15" s="4"/>
       <c r="AF15" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AG15" s="4"/>
       <c r="AH15" s="4">
@@ -2288,7 +2289,7 @@
       <c r="AJ15" s="4"/>
       <c r="AK15" s="4"/>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>7908883300176</v>
       </c>
@@ -2308,7 +2309,7 @@
         <v>21069060</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
@@ -2333,7 +2334,7 @@
         <v>51</v>
       </c>
       <c r="T16" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="U16" s="4"/>
       <c r="V16" s="4"/>
@@ -2363,7 +2364,7 @@
       </c>
       <c r="AE16" s="4"/>
       <c r="AF16" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AG16" s="4"/>
       <c r="AH16" s="4">
@@ -2373,7 +2374,7 @@
       <c r="AJ16" s="4"/>
       <c r="AK16" s="4"/>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>7908883300367</v>
       </c>
@@ -2393,7 +2394,7 @@
         <v>52</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
@@ -2418,7 +2419,7 @@
         <v>51</v>
       </c>
       <c r="T17" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="U17" s="4"/>
       <c r="V17" s="4"/>
@@ -2448,7 +2449,7 @@
       </c>
       <c r="AE17" s="4"/>
       <c r="AF17" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AG17" s="4"/>
       <c r="AH17" s="4">
@@ -2458,7 +2459,7 @@
       <c r="AJ17" s="4"/>
       <c r="AK17" s="4"/>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>7898915380965</v>
       </c>
@@ -2478,7 +2479,7 @@
         <v>52</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
@@ -2503,7 +2504,7 @@
         <v>51</v>
       </c>
       <c r="T18" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="U18" s="4"/>
       <c r="V18" s="4"/>
@@ -2533,7 +2534,7 @@
       </c>
       <c r="AE18" s="4"/>
       <c r="AF18" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AG18" s="4"/>
       <c r="AH18" s="4">
@@ -2543,7 +2544,7 @@
       <c r="AJ18" s="4"/>
       <c r="AK18" s="4"/>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>7898915380019</v>
       </c>
@@ -2552,18 +2553,18 @@
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H19" s="6" t="s">
         <v>52</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
@@ -2590,7 +2591,7 @@
         <v>51</v>
       </c>
       <c r="T19" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="U19" s="4"/>
       <c r="V19" s="4"/>
@@ -2620,7 +2621,7 @@
       </c>
       <c r="AE19" s="4"/>
       <c r="AF19" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AG19" s="4"/>
       <c r="AH19" s="4">
@@ -2630,7 +2631,7 @@
       <c r="AJ19" s="4"/>
       <c r="AK19" s="4"/>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>7898915380033</v>
       </c>
@@ -2639,18 +2640,18 @@
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H20" s="6" t="s">
         <v>52</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
@@ -2677,7 +2678,7 @@
         <v>51</v>
       </c>
       <c r="T20" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="U20" s="4"/>
       <c r="V20" s="4"/>
@@ -2707,7 +2708,7 @@
       </c>
       <c r="AE20" s="4"/>
       <c r="AF20" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AG20" s="4"/>
       <c r="AH20" s="4">
@@ -2717,7 +2718,7 @@
       <c r="AJ20" s="4"/>
       <c r="AK20" s="4"/>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>7898915380057</v>
       </c>
@@ -2726,18 +2727,18 @@
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H21" s="6" t="s">
         <v>52</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
@@ -2764,7 +2765,7 @@
         <v>51</v>
       </c>
       <c r="T21" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U21" s="4"/>
       <c r="V21" s="4"/>
@@ -2794,7 +2795,7 @@
       </c>
       <c r="AE21" s="4"/>
       <c r="AF21" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AG21" s="4"/>
       <c r="AH21" s="4">
@@ -2804,7 +2805,7 @@
       <c r="AJ21" s="4"/>
       <c r="AK21" s="4"/>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>7908883300817</v>
       </c>
@@ -2818,13 +2819,13 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H22" s="6" t="s">
         <v>52</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
@@ -2851,7 +2852,7 @@
         <v>51</v>
       </c>
       <c r="T22" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="U22" s="4"/>
       <c r="V22" s="4"/>
@@ -2881,7 +2882,7 @@
       </c>
       <c r="AE22" s="4"/>
       <c r="AF22" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AG22" s="4"/>
       <c r="AH22" s="4">
@@ -2891,7 +2892,7 @@
       <c r="AJ22" s="4"/>
       <c r="AK22" s="4"/>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>7898915380507</v>
       </c>
@@ -2911,7 +2912,7 @@
         <v>53</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
@@ -2936,7 +2937,7 @@
         <v>51</v>
       </c>
       <c r="T23" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U23" s="4"/>
       <c r="V23" s="4"/>
@@ -2966,7 +2967,7 @@
       </c>
       <c r="AE23" s="4"/>
       <c r="AF23" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AG23" s="4"/>
       <c r="AH23" s="4">
@@ -2976,7 +2977,7 @@
       <c r="AJ23" s="4"/>
       <c r="AK23" s="4"/>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>7898915380514</v>
       </c>
@@ -2996,7 +2997,7 @@
         <v>53</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
@@ -3021,7 +3022,7 @@
         <v>51</v>
       </c>
       <c r="T24" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="U24" s="4"/>
       <c r="V24" s="4"/>
@@ -3051,7 +3052,7 @@
       </c>
       <c r="AE24" s="4"/>
       <c r="AF24" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AG24" s="4"/>
       <c r="AH24" s="4">
@@ -3061,7 +3062,7 @@
       <c r="AJ24" s="4"/>
       <c r="AK24" s="4"/>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>7898915380521</v>
       </c>
@@ -3081,7 +3082,7 @@
         <v>53</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
@@ -3106,7 +3107,7 @@
         <v>51</v>
       </c>
       <c r="T25" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="U25" s="4"/>
       <c r="V25" s="4"/>
@@ -3136,7 +3137,7 @@
       </c>
       <c r="AE25" s="4"/>
       <c r="AF25" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AG25" s="4"/>
       <c r="AH25" s="4">
@@ -3146,7 +3147,7 @@
       <c r="AJ25" s="4"/>
       <c r="AK25" s="4"/>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>7898915380064</v>
       </c>
@@ -3166,7 +3167,7 @@
         <v>53</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
@@ -3193,7 +3194,7 @@
         <v>51</v>
       </c>
       <c r="T26" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="U26" s="4"/>
       <c r="V26" s="4"/>
@@ -3223,7 +3224,7 @@
       </c>
       <c r="AE26" s="4"/>
       <c r="AF26" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AG26" s="4"/>
       <c r="AH26" s="4">
@@ -3233,7 +3234,7 @@
       <c r="AJ26" s="4"/>
       <c r="AK26" s="4"/>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>7898915380811</v>
       </c>
@@ -3253,7 +3254,7 @@
         <v>53</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
@@ -3280,7 +3281,7 @@
         <v>51</v>
       </c>
       <c r="T27" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="U27" s="4"/>
       <c r="V27" s="4"/>
@@ -3310,7 +3311,7 @@
       </c>
       <c r="AE27" s="4"/>
       <c r="AF27" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AG27" s="4"/>
       <c r="AH27" s="4">
@@ -3320,15 +3321,15 @@
       <c r="AJ27" s="4"/>
       <c r="AK27" s="4"/>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="4"/>
       <c r="D28" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F28" s="5">
         <v>2</v>
@@ -3340,7 +3341,7 @@
         <v>53</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
@@ -3368,7 +3369,7 @@
         <v>51</v>
       </c>
       <c r="T28" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="U28" s="4"/>
       <c r="V28" s="4"/>
@@ -3402,7 +3403,7 @@
       <c r="AJ28" s="4"/>
       <c r="AK28" s="4"/>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>7898962720875</v>
       </c>
@@ -3411,18 +3412,18 @@
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H29" s="3">
         <v>21069030</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
@@ -3447,10 +3448,10 @@
         <v>68.040000000000006</v>
       </c>
       <c r="S29" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="T29" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U29" s="4"/>
       <c r="V29" s="4"/>
@@ -3488,7 +3489,7 @@
       <c r="AJ29" s="4"/>
       <c r="AK29" s="4"/>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>7898962720882</v>
       </c>
@@ -3497,18 +3498,18 @@
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H30" s="3">
         <v>21069030</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
@@ -3533,10 +3534,10 @@
         <v>68.040000000000006</v>
       </c>
       <c r="S30" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="T30" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U30" s="4"/>
       <c r="V30" s="4"/>
@@ -3574,7 +3575,7 @@
       <c r="AJ30" s="4"/>
       <c r="AK30" s="4"/>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>7898962720899</v>
       </c>
@@ -3583,18 +3584,18 @@
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H31" s="3">
         <v>21069030</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
@@ -3619,10 +3620,10 @@
         <v>68.040000000000006</v>
       </c>
       <c r="S31" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="T31" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U31" s="4"/>
       <c r="V31" s="4"/>
@@ -3660,7 +3661,7 @@
       <c r="AJ31" s="4"/>
       <c r="AK31" s="4"/>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>7898962720448</v>
       </c>
@@ -3669,18 +3670,18 @@
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H32" s="3">
         <v>21069030</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
@@ -3705,10 +3706,10 @@
         <v>39.744999999999997</v>
       </c>
       <c r="S32" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="T32" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U32" s="4"/>
       <c r="V32" s="4"/>
@@ -3746,7 +3747,7 @@
       <c r="AJ32" s="4"/>
       <c r="AK32" s="4"/>
     </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>7898962720455</v>
       </c>
@@ -3755,18 +3756,18 @@
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H33" s="3">
         <v>21069030</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
@@ -3791,10 +3792,10 @@
         <v>39.744999999999997</v>
       </c>
       <c r="S33" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="T33" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U33" s="4"/>
       <c r="V33" s="4"/>
@@ -3832,7 +3833,7 @@
       <c r="AJ33" s="4"/>
       <c r="AK33" s="4"/>
     </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>7898962720714</v>
       </c>
@@ -3841,18 +3842,18 @@
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H34" s="3">
         <v>21069030</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
@@ -3877,10 +3878,10 @@
         <v>39.744999999999997</v>
       </c>
       <c r="S34" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="T34" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U34" s="4"/>
       <c r="V34" s="4"/>
@@ -3918,7 +3919,7 @@
       <c r="AJ34" s="4"/>
       <c r="AK34" s="4"/>
     </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>7898962720752</v>
       </c>
@@ -3927,18 +3928,18 @@
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H35" s="3">
         <v>21061000</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
@@ -3963,10 +3964,10 @@
         <v>31.68</v>
       </c>
       <c r="S35" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="T35" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U35" s="4"/>
       <c r="V35" s="4"/>
@@ -4004,7 +4005,7 @@
       <c r="AJ35" s="4"/>
       <c r="AK35" s="4"/>
     </row>
-    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>7898962720776</v>
       </c>
@@ -4013,18 +4014,18 @@
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H36" s="3">
         <v>21061000</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
@@ -4049,10 +4050,10 @@
         <v>31.68</v>
       </c>
       <c r="S36" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="T36" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U36" s="4"/>
       <c r="V36" s="4"/>
@@ -4090,7 +4091,7 @@
       <c r="AJ36" s="4"/>
       <c r="AK36" s="4"/>
     </row>
-    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>7898962720790</v>
       </c>
@@ -4099,18 +4100,18 @@
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H37" s="3">
         <v>21061000</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
@@ -4135,10 +4136,10 @@
         <v>31.68</v>
       </c>
       <c r="S37" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="T37" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U37" s="4"/>
       <c r="V37" s="4"/>
@@ -4176,7 +4177,7 @@
       <c r="AJ37" s="4"/>
       <c r="AK37" s="4"/>
     </row>
-    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>7898665680636</v>
       </c>
@@ -4185,12 +4186,12 @@
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H38" s="3">
         <v>20079990</v>
@@ -4221,10 +4222,10 @@
         <v>3.468</v>
       </c>
       <c r="S38" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="T38" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U38" s="4"/>
       <c r="V38" s="4"/>
@@ -4262,7 +4263,7 @@
       <c r="AJ38" s="4"/>
       <c r="AK38" s="4"/>
     </row>
-    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>7898962720349</v>
       </c>
@@ -4271,12 +4272,12 @@
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H39" s="3">
         <v>20081900</v>
@@ -4307,10 +4308,10 @@
         <v>26.01</v>
       </c>
       <c r="S39" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="T39" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U39" s="4"/>
       <c r="V39" s="4"/>
@@ -4348,7 +4349,7 @@
       <c r="AJ39" s="4"/>
       <c r="AK39" s="4"/>
     </row>
-    <row r="40" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>7898962720356</v>
       </c>
@@ -4357,12 +4358,12 @@
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H40" s="3">
         <v>20081900</v>
@@ -4393,10 +4394,10 @@
         <v>26.01</v>
       </c>
       <c r="S40" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="T40" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U40" s="4"/>
       <c r="V40" s="4"/>
@@ -4434,7 +4435,7 @@
       <c r="AJ40" s="4"/>
       <c r="AK40" s="4"/>
     </row>
-    <row r="41" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>7898962720363</v>
       </c>
@@ -4443,12 +4444,12 @@
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
       <c r="G41" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H41" s="3">
         <v>20081900</v>
@@ -4479,10 +4480,10 @@
         <v>26.01</v>
       </c>
       <c r="S41" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="T41" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U41" s="4"/>
       <c r="V41" s="4"/>
@@ -4521,6 +4522,13 @@
       <c r="AK41" s="4"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AK41" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="BALA DE MEL E PROPOLIS"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>